<commit_message>
Added more self-labeled data (improved accuracy); tested self-labeled data gainst itself
</commit_message>
<xml_diff>
--- a/Classification/ClassificationData/Self Labeled Data.xlsx
+++ b/Classification/ClassificationData/Self Labeled Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Uni\DBL Data Challenge\GitLab\Project\dbl-dc-12\Classification\ClassificationData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D086C1B7-F666-4116-9208-FD14FBAAFB3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CCEBD5-C243-41AE-A8DE-04CAD3299159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{458E7466-04A0-4AF8-A19D-7B2E29DE7101}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{458E7466-04A0-4AF8-A19D-7B2E29DE7101}"/>
   </bookViews>
   <sheets>
     <sheet name="TO" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="495">
   <si>
     <t>@VirginAtlantic @Delta @britishairways @Delta do you fancy actually responding to my messages or answering the phone. Been on three occasions for over 3 hours in total and no one picks up at any point. You are ruining our honeymoon. @VirginAtlantic have confirmed the bag was sent yesterday, so where is it! Please help</t>
   </si>
@@ -267,9 +267,6 @@
     <t>DO NOT BOOK WITH @AmericanAir EVER!!!  Their #customerservice is the worst I have ever experienced and given the current circumstances in the DR, they are not even remotely understanding of the situation!!! Again, DO NOT FLY @AmericanAir, they’re AWFUL!!!!</t>
   </si>
   <si>
-    <t>Airline Hate</t>
-  </si>
-  <si>
     <t>@AmericanAir @ELALUSA I checked in for one flight and suddenly I was suddenly checked in for a separate flight and can’t switch seats to sit next to my wife wtf???</t>
   </si>
   <si>
@@ -390,30 +387,15 @@
     <t>@speedbird_uk @UnitedFlyerHD @British_Airways @joelgarabedian @Pilot_Holly @AirbusintheUK The scenery, the plane and the photo. Likely one of the top places to fly and photograph. Amazing.</t>
   </si>
   <si>
-    <t>Hey @British_Airways we are looking forward to Babies first long haul flight this week. We plan to document along the way! Any tips or and thing we should know?! #babysfirstholiday #travellingwithbaby #baby</t>
-  </si>
-  <si>
     <t>@_Alpha_Delta @Dulles_Airport What a great picture, thanks for sharing, Amy! I hope you had a great flight! SamD</t>
   </si>
   <si>
     <t>@abbas_chelsea @SingaporeAir @HeathrowAirport Canon 100-400, but as you can see the picture is cropped. Still quite sharp.</t>
   </si>
   <si>
-    <t>@AmericanAir Congratulations to the happy couple!</t>
-  </si>
-  <si>
     <t>@AvgeekMel @manairport @VirginAtlantic @WaltDisneyWorld WOW that looks so amazing!!! Thanks for sharing!!🤗</t>
   </si>
   <si>
-    <t>@Lowsteppa @easyJet Could you get a soft drink from the Wetherspoons? Lol 😂</t>
-  </si>
-  <si>
-    <t>booked @SingaporeAir ! Yaaaay! Excited for Christmas 🎄 https://t.co/90S0zPAMtE</t>
-  </si>
-  <si>
-    <t>Customer Bonding</t>
-  </si>
-  <si>
     <t>@British_Airways Thanks. Can you please advise on the process of claiming reimbursement for the day of lost work I incurred? (as in, I took Monday off from work, but in reality only flew out Tuesday). Thanks!</t>
   </si>
   <si>
@@ -978,9 +960,6 @@
     <t>@AmericanAir my luggage has been in Atlanta since 3:00 yesterday and you still haven’t delivered to my hotel? It missed 4 delivery runs? How??? Multiple calls...no luggage.</t>
   </si>
   <si>
-    <t>@CardiffOTT @British_Airways Would love to see these and other large aircraft coming into Cardiff daily 🤤🤤 #aviation #planespotting</t>
-  </si>
-  <si>
     <t>@BT77W @BAretrojets @British_Airways @HeathrowAirport Nice capture!</t>
   </si>
   <si>
@@ -1227,9 +1206,6 @@
     <t>@DJKey Hello, great to hear that you're flying with us to Vegas!</t>
   </si>
   <si>
-    <t>They need to implement some strictly followed SOP's or need to improve their automation process.</t>
-  </si>
-  <si>
     <t>@tsandison We can't wait to welcome you on board Trevor! see you soon ^LE</t>
   </si>
   <si>
@@ -1243,16 +1219,325 @@
   </si>
   <si>
     <t>Claims &amp; Refunds</t>
+  </si>
+  <si>
+    <t>Undefined / Unrelated</t>
+  </si>
+  <si>
+    <t>General Complaints &amp; Hate Messages</t>
+  </si>
+  <si>
+    <t>@united YOU SUCK!</t>
+  </si>
+  <si>
+    <t>@united screwing me over twice in one month. Learned my lesson. We are through.</t>
+  </si>
+  <si>
+    <t>@USAirways the least you could do is make up for what you have caused. You are ruining people's memories! You should be ashamed!</t>
+  </si>
+  <si>
+    <t>@united is by far the worst airline ever</t>
+  </si>
+  <si>
+    <t>@united I'm so frustrated and nervous because of this.</t>
+  </si>
+  <si>
+    <t>@AmericanAir has to be the worst airline in the world #yousuck #horrible</t>
+  </si>
+  <si>
+    <t>@USAirways is the worst airline to ever travel with.</t>
+  </si>
+  <si>
+    <t>@AmericanAir are you guys intentionally trying to lose customers and money?</t>
+  </si>
+  <si>
+    <t>@united I hope you lose the next govt contract</t>
+  </si>
+  <si>
+    <t>@VirginAmerica it was a disappointing experience which will be shared with every business traveler I meet. #neverflyvirgin</t>
+  </si>
+  <si>
+    <t>@USAirways i hate you</t>
+  </si>
+  <si>
+    <t>@AmericanAir is the worst airline in the entire world. I only flew them because I had to and it was the nightmare I knew it would be.</t>
+  </si>
+  <si>
+    <t>@JetBlue well, now I'll make sure to never fly JetBlue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @JetBlue u suck Big Donkey Balls!</t>
+  </si>
+  <si>
+    <t>@united Good luck with the no-enertainment-on-6-hour-flights strategy. Innovation at work. Hello @jetblue</t>
+  </si>
+  <si>
+    <t>@SouthwestAir I'm sorry for straying and going with @AmericanAir I've learned my lesson. These attendants need some SW happiness!</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @USAirways this day has been a disaster, rude employees, no help &amp;amp; now no hotel. not flying with you again &amp;amp; I fly ALOT! Dallas=raise=now!</t>
+  </si>
+  <si>
+    <t>@SouthwestAir three hour flight to Orlando and no wifi? Uncool.</t>
+  </si>
+  <si>
+    <t>@AmericanAir pleaseeee find my suitcase. I want deoderant and a clean shirt for work tomorrow :(</t>
+  </si>
+  <si>
+    <t>@united Could you update me on the suitcase please? The online and phone tracking told me nothing. I was told I'd have it back yesterday!</t>
+  </si>
+  <si>
+    <t>@United DO NOT FLY UNITED WITH CHECKED BAGGAGE! It will never find you!</t>
+  </si>
+  <si>
+    <t>@USAirways your flight attendants are all jerks 🐳</t>
+  </si>
+  <si>
+    <t>@united caught earlier flight to ORD. Gate checked bag, and you've lost it at O'Hare. original flight lands in 20minutes. #frustrating!</t>
+  </si>
+  <si>
+    <t>@AmericanAir been waiting in line for over an hour in San Antonio, barely moved &amp;amp; only two agents. 30 in front of me &amp;amp; at least 40 behind.</t>
+  </si>
+  <si>
+    <t>@USAirways 2133. Flight now Cancelled Flightled. Have been rebooked on 2pm flight. If on time take off, I'll have spent 5 extra hours at DCA.</t>
+  </si>
+  <si>
+    <t>@AmericanAir delta rerouted 6 of my bags onto aa977 MIA-CUR. How can I see if they made it onto the flight?</t>
+  </si>
+  <si>
+    <t>@SouthwestAir understood. Just frustrating, you buy early bird check on the day they go on sale at 6:30am and get mid 'b'. Feel ripped off.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @AmericanAir  upon entering plane to 2 @USAirways stewardesses: "can I have some water?" "no we don't do that. please take your seat"</t>
+  </si>
+  <si>
+    <t>@SouthwestAir 45mins wait on the phone with no option for a callback? Finally had to hang up because my phone was dying. #customerservice</t>
+  </si>
+  <si>
+    <t>@USAirways Hey! I booked a flight (Isabelle Gramp, Boston to LAX), and it said that it charged my credit card but the transaction didn't go</t>
+  </si>
+  <si>
+    <t>@AmericanAir been calling 2 different offices already and still no sign of my baggage. First time on American Air..</t>
+  </si>
+  <si>
+    <t>@AmericanAir Still waiting news about my bags 48hrs already happened and this company don't give to the passengers any certain information</t>
+  </si>
+  <si>
+    <t>@SouthwestAir when I called I was told my bag had made it to PHL, but still has not been delivered or any call from the delivery service</t>
+  </si>
+  <si>
+    <t>@SouthwestAir You've inspired me to start my own airline to combat your weak ass airline. sick of this shit</t>
+  </si>
+  <si>
+    <t>@USAirways lack of communication with other offices, the customer, &amp;amp; yall never update ur systems. U guys are 2 established 4 this mess</t>
+  </si>
+  <si>
+    <t>@JetBlue and the 20min line I stood in to drop my bag off?</t>
+  </si>
+  <si>
+    <t>@AmericanAir I've been trying to change a Thursday flight and there's a ridiculous wait time on the phone, and your website isn't helping</t>
+  </si>
+  <si>
+    <t>@SouthwestAir very frustrated with your customer service.Open seats on earlier flight, $154 to change. What a rip off!!</t>
+  </si>
+  <si>
+    <t>@united at MSP w/3 employees trying to check in several hundred and the line is crazy might miss our plane be sure to thank these employees</t>
+  </si>
+  <si>
+    <t>@USAirways @AmericanAir 2hrs Late Flightr finally taking off😂😂😂</t>
+  </si>
+  <si>
+    <t>@VirginAmerica trying to book a flight &amp;amp; your site is down 😁</t>
+  </si>
+  <si>
+    <t>@SouthwestAir Open more kiosks at \r\nAustin-Bergstrom. Three lanes to service a line of 50 people? Really?</t>
+  </si>
+  <si>
+    <t>@AmericanAir why do you continually play the "according to federal regulations" every 58 seconds. I could see if you had quicker service...</t>
+  </si>
+  <si>
+    <t>@USAirways Hey. I hve Cancelled Flightled flght &amp;amp; on hold for 30 min nw 4 rebook. Website not working. Can u give me some insight if I DM conf #?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @united it's not there we tried. It's already here in cancun just no one has delivered it</t>
+  </si>
+  <si>
+    <t>@AmericanAir was told at 7pm my bags would 1000% be at my house by 9pm. Well they're not and I continue to be lied to.</t>
+  </si>
+  <si>
+    <t>@united I'm in Denver, my bag is in San Jose. See something wrong here.</t>
+  </si>
+  <si>
+    <t>@united the bag is in a state that I didn't travel to and the airports don't fly to each other. Looks like it'll never show</t>
+  </si>
+  <si>
+    <t>@USAirways Hi. I'm in LGA but my luggage is in CLT. Have been told to come back tomorrow to collect. Do you guys want to cover my taxi fare?</t>
+  </si>
+  <si>
+    <t>@AmericanAir why won't u deliver my luggage? Almost two days and holding on the phone for over 4 hrs. Help!</t>
+  </si>
+  <si>
+    <t>@USAirways you have the ability to switch my flight to @AmericanAir but you cannot tell me where my bags are.</t>
+  </si>
+  <si>
+    <t>@united Our flight was originally supposed to leave at 1:40pm &amp;amp; now we won't leave until 5. This is the 2nd time this has happened</t>
+  </si>
+  <si>
+    <t>@united Flight 6212...massive fail! They delaying to transport a crew member causing many to miss connections! Unreal!</t>
+  </si>
+  <si>
+    <t>@united are you trying to break a world record for most delayed flights in a year?</t>
+  </si>
+  <si>
+    <t>@AmericanAir Oh, and losing my luggage #ridiculous # angrybird # where'smybag</t>
+  </si>
+  <si>
+    <t>@AmericanAir not sure why we are being made to stand in line outside for plane that isn't ready to board when I could be sitting inside</t>
+  </si>
+  <si>
+    <t>@united I have tried and you have failed. Still no wifi ever, last row in the middle and I fly every week. Thanks for nothing.</t>
+  </si>
+  <si>
+    <t>@AmericanAir I certainly hope my LA /PBI on 25 th has a NEW plane . The seats on Feb 11 th flight ( in reverse) God awful</t>
+  </si>
+  <si>
+    <t>@AmericanAir @dogbuckeye No, I was on hold for 4 1/2 hours.  3 diff agents each w/ different information, frustrating, kept getting txfd...</t>
+  </si>
+  <si>
+    <t>@USAirways I have been trying to book a flight using my miles for 3 straight days. 210 min on phone - still haven't talked to a human.</t>
+  </si>
+  <si>
+    <t>@USAirways i dont need to check status of my flight because i was ON the plane and you had a door malfunction. Get it together!!</t>
+  </si>
+  <si>
+    <t>@united since bulkhead seats cannot have bags on floor, why don't u reserve o/head space above those seats? In 1B on UA246 - not impressed</t>
+  </si>
+  <si>
+    <t>@USAirways and yet the Flight Attendant argued with me over Exec Plat benefits...</t>
+  </si>
+  <si>
+    <t>@USAirways it is really embarrassing when asking for complimentary drink/snack detailed here: https://t.co/9zA6xb1h89 &amp;amp; being argued with.</t>
+  </si>
+  <si>
+    <t>@WoodhouseAlice Thanks very much for sharing, Alice! Jera</t>
+  </si>
+  <si>
+    <t>@LamekeB That's great news, Chris. We're so glad our team was able to assist you during your flight.</t>
+  </si>
+  <si>
+    <t>@travisloop Isn't that neat? We're glad you're enjoying your time and appreciate you flying with us!</t>
+  </si>
+  <si>
+    <t>@British_Airways  dear @British_Airways I think I have a problem with my executive club membership, it looks like I’ve been charged twice for some purchases I made with my avios in the wine club. Is there an email address I can use to enquire?</t>
+  </si>
+  <si>
+    <t>Just had to pay a ransom to @AmericanAir so my miles wouldn’t expire. Airline miles are savings that should be passed along to customers at the transaction, not some non taxable banana republic gold reserve governed by predatory central bank policies!!!!!!!</t>
+  </si>
+  <si>
+    <t>Thanks @easyJet another weekend off to a delayed start thanks to you. My friend wants someone to arrange a party in a local brewery. Are you free? Oh, wait ...</t>
+  </si>
+  <si>
+    <t>Hey @AmericanAir - you delayed my flight by 2 hours, caused me to miss my connection, had multiple agents give me incorrect information, and now it’s 11:26pm and I’m stranded at the airport and expected to be in Grand Rapids tomorrow at 9 for work. How are you going to fix it?</t>
+  </si>
+  <si>
+    <t>@easyJet stuck in Bologna as your flight for tomorrow is cancelled. Live and work in UK and I wonder if there is any way you are taking Britons  back home. Flights are only available at the end of the month, cannot wait so long!  How can I find a solution, please? Thank you</t>
+  </si>
+  <si>
+    <t>Update: @AmericanAir you still don’t have a captain and one isn’t showing up for a couple hours. Crushing it out of the park!</t>
+  </si>
+  <si>
+    <t>@easyJet Day 3 of trying to get someone from easyJet to look at my cancellation refund request. Any chance of success today!?</t>
+  </si>
+  <si>
+    <t>@TheTomMac @Ryanair @TheTomMac did you manage to get anywhere with your query RE cancelling and getting a refund?</t>
+  </si>
+  <si>
+    <t>@G__Nev @Ryanair I had exactly the same experience.. I changed my flights for FREE.. I ended up paying more for cheaper flights 🤔</t>
+  </si>
+  <si>
+    <t>@mbrodwell @British_Airways I’d switch to @VirginAtlantic far better fleet, app, service &amp;amp; pricing. I’d rather swim than endure BA attitude</t>
+  </si>
+  <si>
+    <t>@Wasie21 Hi there. I can't explain the difference between £119 and £99. However, an infant pays 10% of an adult fare plus taxes. The taxes aren't equal to 10% of an adult tax, hence why the cost won't be £59.60/ PhilGW</t>
+  </si>
+  <si>
+    <t>@orange1gman Prices out in 23rd via places aren't too bad, 25th are expensive, I'm on Ryanair &amp;amp; easyJet trying to plot a route</t>
+  </si>
+  <si>
+    <t>Like big props to Qantas for the free pass but honestly only boomers would pay literally hundreds of dollars a year to eat tinned peaches or Arnott's biscuits in a separate room from the rest of the airport</t>
+  </si>
+  <si>
+    <t>@AmericanAir @andrewkimmel Still cheaper than the nearly $2k they wanted you to pay, and now you can write a movie about your ordeal. “Frequent Flyer”.</t>
+  </si>
+  <si>
+    <t>@dannydevitno Skyscanner, but check easyJet and KLM’s sites directly cus might have Black Friday sales, I got £40 return to Warsaw x</t>
+  </si>
+  <si>
+    <t>@British_Airways thanks BA pay 50 euro for a seat so i can leave aircraft early. Had to stick hand baggage in row 34. Means i will be last off plane . #ripoff</t>
+  </si>
+  <si>
+    <t>I flew @KLM from Amsterdam to Helsinki this morning and look what the cabin crew gave me! Such a nice way to make my birthday a bit more special. Thank you! ❤</t>
+  </si>
+  <si>
+    <t>@BorisKodjoe @AmericanAir They must have the worse flight attendants. It seems I read a different post about their rudeness and very poor customer service almost every week!</t>
+  </si>
+  <si>
+    <t>@AmericanAir Your flight attendant Kirani (apologies if my spelling is off) was the epitome of class and customer service and I just wanted to recognize her. MAJOR kudos to her. Flight AA 2645 LGA-MCO.</t>
+  </si>
+  <si>
+    <t>@British_Airways Not able to check in for my flights tomorrow via the app or web site - can u help?</t>
+  </si>
+  <si>
+    <t>@British_Airways really disappointed to have booked my flghts only to call over 20 times and try to sort out seats only to be told by an automated system that your too busy to take my call then it just hangs up! really unhappy with this.</t>
+  </si>
+  <si>
+    <t>@puneetnagpal06 @lufthansa @Lufthansa_India @DelhiAirport @MoCA_GoI This is everywhere in the world with Lufthansa apparently, they are worst than a low cost airline. How come do they stay among the top airlines ... not a single idea ... maybe the top at profits for sure !!</t>
+  </si>
+  <si>
+    <t>@sandoshi786 @EtihadAirways @EtihadHelp It is a nightmare. Never traveling #etihad again.</t>
+  </si>
+  <si>
+    <t>@SingaporeAir Thank you!!</t>
+  </si>
+  <si>
+    <t>@SingaporeAir @SingaporeAir thank you for your assistance and swift approach! Appreciate it!</t>
+  </si>
+  <si>
+    <t>@AmericanAir Being a Million Mile and Platinum Member is worthless! #gavemyseataway#bumped my flight!#Awful customer service!!!!</t>
+  </si>
+  <si>
+    <t>Plus no response from bombay lufthansa staff. They dint even pick up phones. Worst service.</t>
+  </si>
+  <si>
+    <t>@easyJet I always believe in posting good stuff as well as bad so today I wanted to say a big thank you for your excellent customer service I received when calling up your call centre to make a change on behalf of my daughter who is many thousands of miles away in China....</t>
+  </si>
+  <si>
+    <t>@TheForwardCabin The gate agent with @AmericanAir at DFW YELLED at me that I needed to hurry &amp;amp; get my dog in her carrier so I could board even though it was obvious I was having problems getting her in even though I had given her an anti-anxiety pill. Their yelling did NOTHING to help.</t>
+  </si>
+  <si>
+    <t>When passion is your super power, your dreams are limitless. Meet Qistina, this is her story. #Etihad</t>
+  </si>
+  <si>
+    <t>@DunkItDecker @luka7doncic @lufthansa Let me guess.  You went to the Sanders School of Mathematics 🧮?</t>
+  </si>
+  <si>
+    <t>@ShamaSrujan @CowboyExpat @jcasavant @steelersfanOG @BravoAndy @AmericanAir And yet, when you walk into someone else's space, if they punch you, by your own thought process above, you'd be fine with that.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1278,8 +1563,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1594,10 +1882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDF4DF03-31AE-4140-A489-DD3AAC4A025E}">
-  <dimension ref="A1:B313"/>
+  <dimension ref="A1:B404"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A315" sqref="A315"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="K424" sqref="K424"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1987,7 +2275,7 @@
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1995,7 +2283,7 @@
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2003,7 +2291,7 @@
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2011,7 +2299,7 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2019,7 +2307,7 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2027,7 +2315,7 @@
         <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2035,7 +2323,7 @@
         <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2043,7 +2331,7 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2051,7 +2339,7 @@
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2059,7 +2347,7 @@
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2067,7 +2355,7 @@
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2075,7 +2363,7 @@
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -2083,7 +2371,7 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2091,7 +2379,7 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2099,7 +2387,7 @@
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2107,7 +2395,7 @@
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2115,7 +2403,7 @@
         <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>76</v>
+        <v>395</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2123,7 +2411,7 @@
         <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>76</v>
+        <v>395</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2131,7 +2419,7 @@
         <v>68</v>
       </c>
       <c r="B66" t="s">
-        <v>76</v>
+        <v>395</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2139,7 +2427,7 @@
         <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>76</v>
+        <v>395</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -2147,7 +2435,7 @@
         <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>76</v>
+        <v>395</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2155,7 +2443,7 @@
         <v>71</v>
       </c>
       <c r="B69" t="s">
-        <v>76</v>
+        <v>392</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2163,7 +2451,7 @@
         <v>72</v>
       </c>
       <c r="B70" t="s">
-        <v>76</v>
+        <v>395</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -2171,7 +2459,7 @@
         <v>73</v>
       </c>
       <c r="B71" t="s">
-        <v>76</v>
+        <v>395</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -2179,7 +2467,7 @@
         <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>76</v>
+        <v>395</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -2187,351 +2475,351 @@
         <v>75</v>
       </c>
       <c r="B73" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B78" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B79" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B81" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B82" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B83" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B84" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B85" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B86" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B87" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B88" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B89" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B90" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B91" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B92" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B93" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B94" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>98</v>
+      </c>
+      <c r="B95" t="s">
         <v>99</v>
-      </c>
-      <c r="B95" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B96" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B97" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B98" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B99" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B100" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B101" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B102" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B103" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>108</v>
+      </c>
+      <c r="B104" t="s">
         <v>109</v>
-      </c>
-      <c r="B104" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B105" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B106" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B107" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B108" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B109" t="s">
-        <v>124</v>
+        <v>392</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B110" t="s">
-        <v>124</v>
+        <v>392</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B111" t="s">
-        <v>124</v>
+        <v>392</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B112" t="s">
-        <v>124</v>
+        <v>392</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B113" t="s">
-        <v>124</v>
+        <v>48</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B114" t="s">
-        <v>124</v>
+        <v>393</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B115" t="s">
-        <v>124</v>
+        <v>393</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="B116" t="s">
-        <v>124</v>
+        <v>393</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -2539,31 +2827,31 @@
         <v>123</v>
       </c>
       <c r="B117" t="s">
-        <v>124</v>
+        <v>393</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B118" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B119" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="B120" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -2571,7 +2859,7 @@
         <v>129</v>
       </c>
       <c r="B121" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -2579,215 +2867,215 @@
         <v>130</v>
       </c>
       <c r="B122" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B123" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="B124" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B125" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B126" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B127" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B128" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B129" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B130" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B131" t="s">
-        <v>401</v>
+        <v>145</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="B132" t="s">
-        <v>401</v>
+        <v>145</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
+        <v>126</v>
+      </c>
+      <c r="B133" t="s">
         <v>145</v>
-      </c>
-      <c r="B133" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>144</v>
+        <v>121</v>
       </c>
       <c r="B134" t="s">
-        <v>401</v>
+        <v>145</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="B135" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B136" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B137" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B138" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="B139" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="B140" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="B141" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="B142" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B143" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B144" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B145" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="B146" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="B147" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="B148" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
@@ -2795,23 +3083,23 @@
         <v>152</v>
       </c>
       <c r="B149" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B150" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B151" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
@@ -2819,39 +3107,39 @@
         <v>157</v>
       </c>
       <c r="B152" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B153" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B154" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B155" t="s">
-        <v>168</v>
+        <v>394</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B156" t="s">
-        <v>168</v>
+        <v>394</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
@@ -2859,132 +3147,132 @@
         <v>165</v>
       </c>
       <c r="B157" t="s">
-        <v>168</v>
+        <v>394</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B158" t="s">
-        <v>168</v>
+        <v>394</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B159" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B160" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B161" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B162" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B163" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B164" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B165" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B166" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B167" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B168" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>179</v>
+        <v>218</v>
       </c>
       <c r="B169" t="s">
-        <v>223</v>
+        <v>36</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>180</v>
+        <v>219</v>
       </c>
       <c r="B170" t="s">
-        <v>223</v>
+        <v>36</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>181</v>
+        <v>220</v>
       </c>
       <c r="B171" t="s">
-        <v>223</v>
+        <v>36</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>182</v>
+        <v>221</v>
       </c>
       <c r="B172" t="s">
-        <v>183</v>
+        <v>36</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B173" t="s">
         <v>36</v>
@@ -2992,7 +3280,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B174" t="s">
         <v>36</v>
@@ -3000,7 +3288,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B175" t="s">
         <v>36</v>
@@ -3008,7 +3296,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B176" t="s">
         <v>36</v>
@@ -3016,7 +3304,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B177" t="s">
         <v>36</v>
@@ -3024,7 +3312,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B178" t="s">
         <v>36</v>
@@ -3032,7 +3320,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B179" t="s">
         <v>36</v>
@@ -3040,7 +3328,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B180" t="s">
         <v>36</v>
@@ -3048,7 +3336,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B181" t="s">
         <v>36</v>
@@ -3056,7 +3344,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B182" t="s">
         <v>36</v>
@@ -3064,7 +3352,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B183" t="s">
         <v>36</v>
@@ -3072,39 +3360,39 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B184" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B185" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B186" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B187" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B188" t="s">
         <v>48</v>
@@ -3112,7 +3400,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B189" t="s">
         <v>48</v>
@@ -3120,7 +3408,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B190" t="s">
         <v>48</v>
@@ -3128,999 +3416,1728 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B191" t="s">
-        <v>48</v>
+        <v>392</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B192" t="s">
-        <v>48</v>
+        <v>392</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B193" t="s">
-        <v>48</v>
+        <v>392</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B194" t="s">
-        <v>48</v>
+        <v>392</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B195" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B196" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B197" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B198" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B199" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B200" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B201" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B202" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B203" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B204" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B205" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B206" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B207" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B208" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B209" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B210" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B211" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B212" t="s">
-        <v>76</v>
+        <v>395</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B213" t="s">
-        <v>76</v>
+        <v>262</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B214" t="s">
-        <v>76</v>
+        <v>262</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B215" t="s">
-        <v>76</v>
+        <v>262</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B216" t="s">
-        <v>76</v>
+        <v>262</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B217" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B218" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B219" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B220" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B221" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B222" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B223" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B224" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B225" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B226" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B227" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B228" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B229" t="s">
-        <v>268</v>
+        <v>99</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B230" t="s">
-        <v>268</v>
+        <v>99</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B231" t="s">
-        <v>268</v>
+        <v>99</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B232" t="s">
-        <v>268</v>
+        <v>99</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B233" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B234" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B235" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B236" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B237" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B238" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B239" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B240" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B241" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B242" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B243" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B244" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B245" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B246" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B247" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B248" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B249" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B250" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B251" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B252" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B253" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B254" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B255" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B256" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B257" t="s">
-        <v>110</v>
+        <v>392</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B258" t="s">
-        <v>110</v>
+        <v>392</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B259" t="s">
-        <v>110</v>
+        <v>393</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B260" t="s">
-        <v>110</v>
+        <v>393</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B261" t="s">
-        <v>124</v>
+        <v>393</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B262" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B263" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B264" t="s">
-        <v>401</v>
+        <v>145</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B265" t="s">
-        <v>401</v>
+        <v>145</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B266" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B267" t="s">
-        <v>151</v>
+        <v>393</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B268" t="s">
-        <v>151</v>
+        <v>393</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B269" t="s">
-        <v>151</v>
+        <v>393</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B270" t="s">
-        <v>151</v>
+        <v>393</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B271" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B272" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B273" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B274" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B275" t="s">
-        <v>401</v>
+        <v>145</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B276" t="s">
-        <v>401</v>
+        <v>145</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B277" t="s">
-        <v>401</v>
+        <v>145</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B278" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B279" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B280" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B281" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B282" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B283" t="s">
-        <v>401</v>
+        <v>162</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B284" t="s">
-        <v>401</v>
+        <v>162</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B285" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B286" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B287" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B288" t="s">
-        <v>168</v>
+        <v>394</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B289" t="s">
-        <v>168</v>
+        <v>394</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B290" t="s">
-        <v>168</v>
+        <v>394</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B291" t="s">
-        <v>168</v>
+        <v>394</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B292" t="s">
-        <v>168</v>
+        <v>394</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B293" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B294" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B295" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B296" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B297" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B298" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B299" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B300" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B301" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B302" t="s">
-        <v>223</v>
+        <v>394</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B303" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B304" t="s">
-        <v>223</v>
+        <v>359</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B305" t="s">
-        <v>223</v>
+        <v>359</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B306" t="s">
-        <v>223</v>
+        <v>359</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
+        <v>357</v>
+      </c>
+      <c r="B307" t="s">
         <v>359</v>
-      </c>
-      <c r="B307" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B308" t="s">
-        <v>183</v>
+        <v>359</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A309" t="s">
-        <v>361</v>
+      <c r="A309" s="1" t="s">
+        <v>396</v>
       </c>
       <c r="B309" t="s">
-        <v>366</v>
+        <v>395</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A310" t="s">
-        <v>362</v>
+      <c r="A310" s="1" t="s">
+        <v>401</v>
       </c>
       <c r="B310" t="s">
-        <v>366</v>
+        <v>395</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A311" t="s">
-        <v>363</v>
+      <c r="A311" s="1" t="s">
+        <v>397</v>
       </c>
       <c r="B311" t="s">
-        <v>366</v>
+        <v>395</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A312" t="s">
-        <v>364</v>
+      <c r="A312" s="1" t="s">
+        <v>398</v>
       </c>
       <c r="B312" t="s">
-        <v>366</v>
+        <v>395</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A313" t="s">
-        <v>365</v>
+      <c r="A313" s="1" t="s">
+        <v>399</v>
       </c>
       <c r="B313" t="s">
-        <v>366</v>
+        <v>395</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A314" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B314" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A315" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B315" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A316" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B316" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A317" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B317" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A318" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B318" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A319" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B319" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A320" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B320" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A321" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="B321" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A322" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B322" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A323" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B323" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A324" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B324" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A325" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B325" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A326" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B326" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A327" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="B327" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A328" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B328" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A329" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B329" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A330" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B330" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A331" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B331" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A332" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B332" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A333" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B333" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A334" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B334" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A335" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B335" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A336" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B336" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A337" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B337" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A338" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B338" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A339" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B339" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A340" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B340" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A341" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="B341" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A342" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B342" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A343" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B343" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A344" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B344" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A345" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B345" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A346" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B346" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A347" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B347" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A348" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B348" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A349" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B349" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A350" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B350" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A351" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B351" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A352" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B352" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A353" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B353" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A354" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B354" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A355" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B355" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A356" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B356" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A357" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B357" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A358" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B358" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A359" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B359" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A360" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="B360" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A361" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B361" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A362" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B362" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A363" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B363" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A364" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B364" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A365" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="B365" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A366" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B366" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A367" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B367" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A368" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="B368" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A369" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B369" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A370" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B370" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A371" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B371" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A372" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B372" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>463</v>
+      </c>
+      <c r="B373" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>464</v>
+      </c>
+      <c r="B374" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>465</v>
+      </c>
+      <c r="B375" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>466</v>
+      </c>
+      <c r="B376" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>467</v>
+      </c>
+      <c r="B377" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
+        <v>468</v>
+      </c>
+      <c r="B378" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>469</v>
+      </c>
+      <c r="B379" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>470</v>
+      </c>
+      <c r="B380" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>471</v>
+      </c>
+      <c r="B381" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>472</v>
+      </c>
+      <c r="B382" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>473</v>
+      </c>
+      <c r="B383" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>474</v>
+      </c>
+      <c r="B384" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>475</v>
+      </c>
+      <c r="B385" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>476</v>
+      </c>
+      <c r="B386" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>477</v>
+      </c>
+      <c r="B387" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>478</v>
+      </c>
+      <c r="B388" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>479</v>
+      </c>
+      <c r="B389" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>480</v>
+      </c>
+      <c r="B390" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>481</v>
+      </c>
+      <c r="B391" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>482</v>
+      </c>
+      <c r="B392" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>483</v>
+      </c>
+      <c r="B393" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>484</v>
+      </c>
+      <c r="B394" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>485</v>
+      </c>
+      <c r="B395" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>486</v>
+      </c>
+      <c r="B396" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>487</v>
+      </c>
+      <c r="B397" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>488</v>
+      </c>
+      <c r="B398" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A399" t="s">
+        <v>489</v>
+      </c>
+      <c r="B399" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
+        <v>490</v>
+      </c>
+      <c r="B400" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>491</v>
+      </c>
+      <c r="B401" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
+        <v>492</v>
+      </c>
+      <c r="B402" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>493</v>
+      </c>
+      <c r="B403" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>494</v>
+      </c>
+      <c r="B404" t="s">
+        <v>394</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1776599D-50A0-4C05-B448-436B301DBFF1}">
-  <dimension ref="A1:B72"/>
+  <dimension ref="A1:B119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67:B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4130,7 +5147,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B1" t="s">
         <v>36</v>
@@ -4138,7 +5155,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
@@ -4146,7 +5163,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
@@ -4154,7 +5171,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B4" t="s">
         <v>36</v>
@@ -4162,7 +5179,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B5" t="s">
         <v>36</v>
@@ -4170,7 +5187,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
@@ -4178,7 +5195,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="B7" t="s">
         <v>36</v>
@@ -4186,7 +5203,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B8" t="s">
         <v>36</v>
@@ -4194,7 +5211,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="B9" t="s">
         <v>36</v>
@@ -4202,7 +5219,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B10" t="s">
         <v>36</v>
@@ -4210,7 +5227,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
@@ -4218,7 +5235,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
@@ -4226,7 +5243,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B13" t="s">
         <v>36</v>
@@ -4234,7 +5251,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="B14" t="s">
         <v>36</v>
@@ -4242,7 +5259,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B15" t="s">
         <v>65</v>
@@ -4250,103 +5267,103 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="B24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="B27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B28" t="s">
         <v>48</v>
@@ -4354,7 +5371,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B29" t="s">
         <v>48</v>
@@ -4362,7 +5379,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B30" t="s">
         <v>48</v>
@@ -4370,7 +5387,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B31" t="s">
         <v>48</v>
@@ -4378,7 +5395,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B32" t="s">
         <v>48</v>
@@ -4386,7 +5403,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B33" t="s">
         <v>48</v>
@@ -4394,7 +5411,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B34" t="s">
         <v>48</v>
@@ -4402,79 +5419,79 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B35" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B36" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B37" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B38" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B39" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="B40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="B41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B42" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="B43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="B44" t="s">
         <v>36</v>
@@ -4482,7 +5499,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="B45" t="s">
         <v>36</v>
@@ -4490,7 +5507,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="B46" t="s">
         <v>36</v>
@@ -4498,7 +5515,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="B47" t="s">
         <v>36</v>
@@ -4506,119 +5523,119 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="B48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="B49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="B50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="B51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="B52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="B53" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="B54" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B55" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="B56" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B57" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="B58" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B59" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="B60" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B61" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="B62" t="s">
         <v>65</v>
@@ -4626,7 +5643,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="B63" t="s">
         <v>65</v>
@@ -4634,7 +5651,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="B64" t="s">
         <v>65</v>
@@ -4642,7 +5659,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="B65" t="s">
         <v>65</v>
@@ -4650,7 +5667,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B66" t="s">
         <v>48</v>
@@ -4658,7 +5675,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B67" t="s">
         <v>48</v>
@@ -4666,7 +5683,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="B68" t="s">
         <v>48</v>
@@ -4674,7 +5691,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="B69" t="s">
         <v>48</v>
@@ -4682,7 +5699,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>397</v>
+        <v>460</v>
       </c>
       <c r="B70" t="s">
         <v>48</v>
@@ -4690,7 +5707,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>398</v>
+        <v>461</v>
       </c>
       <c r="B71" t="s">
         <v>48</v>
@@ -4698,10 +5715,250 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>399</v>
+        <v>462</v>
       </c>
       <c r="B72" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>116</v>
+      </c>
+      <c r="B73" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>391</v>
+      </c>
+      <c r="B74" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>387</v>
+      </c>
+      <c r="B75" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>116</v>
+      </c>
+      <c r="B93" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>391</v>
+      </c>
+      <c r="B94" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>387</v>
+      </c>
+      <c r="B95" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>390</v>
+      </c>
+      <c r="B96" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>460</v>
+      </c>
+      <c r="B97" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>461</v>
+      </c>
+      <c r="B98" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>462</v>
+      </c>
+      <c r="B99" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>388</v>
+      </c>
+      <c r="B100" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>378</v>
+      </c>
+      <c r="B101" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>379</v>
+      </c>
+      <c r="B102" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>381</v>
+      </c>
+      <c r="B103" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>210</v>
+      </c>
+      <c r="B104" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>211</v>
+      </c>
+      <c r="B105" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>213</v>
+      </c>
+      <c r="B106" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>214</v>
+      </c>
+      <c r="B107" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>215</v>
+      </c>
+      <c r="B108" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>208</v>
+      </c>
+      <c r="B109" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>196</v>
+      </c>
+      <c r="B110" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>197</v>
+      </c>
+      <c r="B111" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>198</v>
+      </c>
+      <c r="B112" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>199</v>
+      </c>
+      <c r="B113" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>204</v>
+      </c>
+      <c r="B114" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>205</v>
+      </c>
+      <c r="B115" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>206</v>
+      </c>
+      <c r="B116" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>368</v>
+      </c>
+      <c r="B117" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>369</v>
+      </c>
+      <c r="B118" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>370</v>
+      </c>
+      <c r="B119" t="s">
+        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>